<commit_message>
Removed data quality in excel / added it as the log 💅
</commit_message>
<xml_diff>
--- a/processed_rent_roll.xlsx
+++ b/processed_rent_roll.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Processed Rent Roll" sheetId="1" r:id="rId1"/>
-    <sheet name="Validation Errors" sheetId="2" r:id="rId2"/>
-    <sheet name="Data Quality Metrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4357" uniqueCount="1653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="1632">
   <si>
     <t>Resh ID</t>
   </si>
@@ -4912,69 +4910,6 @@
   </si>
   <si>
     <t>1,825.00</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>missing_columns</t>
-  </si>
-  <si>
-    <t>Empty values in rows: [225]</t>
-  </si>
-  <si>
-    <t>occupancy_status</t>
-  </si>
-  <si>
-    <t>tenant_name</t>
-  </si>
-  <si>
-    <t>lease_term</t>
-  </si>
-  <si>
-    <t>Metric</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>total_rows</t>
-  </si>
-  <si>
-    <t>missing_values_by_column</t>
-  </si>
-  <si>
-    <t>completeness_ratio</t>
-  </si>
-  <si>
-    <t>duplicate_rows</t>
-  </si>
-  <si>
-    <t>columns_found</t>
-  </si>
-  <si>
-    <t>columns_mapped</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>{'Resh ID': 0, 'Lease ID': 14, 'unit': 1, 'unit_type': 0, 'Unit Designation': 0, 'sq_ft': 1, 'Unit/Lease Status': 0, 'Name': 0, 'Phone Number': 0, 'Email': 0, 'move_in_date': 0, 'Notice For Date': 0, 'lease_start': 0, 'lease_end': 0, 'Market + Addl.': 0, 'Dep On Hand': 0, 'Balance': 0, 'Total Charges': 0, 'contract_rent': 0, 'PEST                          ': 0, 'VALET TRASH                   ': 0, 'TRASH                         ': 0, 'PETRENT                       ': 0, 'LOP15                         ': 0, 'EMPLCRED                      ': 0, 'OHIOCHOICE                    ': 0, 'WAIVED ADMIN FEE              ': 0, 'WAIVED APP FEE                ': 0, 'SETUPFEE                      ': 0}</t>
-  </si>
-  <si>
-    <t>0.9975478927203065</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>['Resh ID', 'Lease ID', 'unit', 'unit_type', 'Unit Designation', 'sq_ft', 'Unit/Lease Status', 'Name', 'Phone Number', 'Email', 'move_in_date', 'Notice For Date', 'lease_start', 'lease_end', 'Market + Addl.', 'Dep On Hand', 'Balance', 'Total Charges', 'contract_rent', 'PEST                          ', 'VALET TRASH                   ', 'TRASH                         ', 'PETRENT                       ', 'LOP15                         ', 'EMPLCRED                      ', 'OHIOCHOICE                    ', 'WAIVED ADMIN FEE              ', 'WAIVED APP FEE                ', 'SETUPFEE                      ']</t>
-  </si>
-  <si>
-    <t>['unit', 'contract_rent', 'lease_start', 'unit_type', 'lease_end', 'sq_ft', 'move_in_date']</t>
   </si>
 </sst>
 </file>
@@ -5044,16 +4979,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -25445,126 +25377,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1635</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1642</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1648</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>1645</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1651</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>1646</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>